<commit_message>
Estimation of length and weight at 1st spawning (farm only)
</commit_message>
<xml_diff>
--- a/Age at hatching data.xlsx
+++ b/Age at hatching data.xlsx
@@ -4376,7 +4376,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4671,11 +4671,11 @@
         <v>255</v>
       </c>
       <c r="D2">
-        <f>1/B2</f>
+        <f t="shared" ref="D2:D23" si="0">1/B2</f>
         <v>3.6583135174684477E-3</v>
       </c>
       <c r="E2">
-        <f>LOG(1/C2)</f>
+        <f t="shared" ref="E2:E23" si="1">LOG(1/C2)</f>
         <v>-2.406540180433955</v>
       </c>
     </row>
@@ -4684,18 +4684,18 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B23" si="0">A3+273.15</f>
+        <f t="shared" ref="B3:B23" si="2">A3+273.15</f>
         <v>274.14999999999998</v>
       </c>
       <c r="C3">
         <v>210.75</v>
       </c>
       <c r="D3">
-        <f>1/B3</f>
+        <f t="shared" si="0"/>
         <v>3.6476381542950944E-3</v>
       </c>
       <c r="E3">
-        <f>LOG(1/C3)</f>
+        <f t="shared" si="1"/>
         <v>-2.3237675832967799</v>
       </c>
     </row>
@@ -4704,18 +4704,18 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>275.14999999999998</v>
       </c>
       <c r="C4">
         <v>157</v>
       </c>
       <c r="D4">
-        <f>1/B4</f>
+        <f t="shared" si="0"/>
         <v>3.6343812465927678E-3</v>
       </c>
       <c r="E4">
-        <f>LOG(1/C4)</f>
+        <f t="shared" si="1"/>
         <v>-2.1958996524092336</v>
       </c>
     </row>
@@ -4724,18 +4724,18 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>277.14999999999998</v>
       </c>
       <c r="C5">
         <v>123</v>
       </c>
       <c r="D5">
-        <f>1/B5</f>
+        <f t="shared" si="0"/>
         <v>3.608154429009562E-3</v>
       </c>
       <c r="E5">
-        <f>LOG(1/C5)</f>
+        <f t="shared" si="1"/>
         <v>-2.0899051114393981</v>
       </c>
     </row>
@@ -4744,18 +4744,18 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>279.14999999999998</v>
       </c>
       <c r="C6">
         <v>83</v>
       </c>
       <c r="D6">
-        <f>1/B6</f>
+        <f t="shared" si="0"/>
         <v>3.5823034210997673E-3</v>
       </c>
       <c r="E6">
-        <f>LOG(1/C6)</f>
+        <f t="shared" si="1"/>
         <v>-1.919078092376074</v>
       </c>
     </row>
@@ -4764,18 +4764,18 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>281.14999999999998</v>
       </c>
       <c r="C7">
         <v>62</v>
       </c>
       <c r="D7">
-        <f>1/B7</f>
+        <f t="shared" si="0"/>
         <v>3.556820202738752E-3</v>
       </c>
       <c r="E7">
-        <f>LOG(1/C7)</f>
+        <f t="shared" si="1"/>
         <v>-1.7923916894982539</v>
       </c>
     </row>
@@ -4784,18 +4784,18 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>283.14999999999998</v>
       </c>
       <c r="C8">
         <v>50</v>
       </c>
       <c r="D8">
-        <f>1/B8</f>
+        <f t="shared" si="0"/>
         <v>3.5316969803990822E-3</v>
       </c>
       <c r="E8">
-        <f>LOG(1/C8)</f>
+        <f t="shared" si="1"/>
         <v>-1.6989700043360187</v>
       </c>
     </row>
@@ -4804,18 +4804,18 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>285.14999999999998</v>
       </c>
       <c r="C9">
         <v>40</v>
       </c>
       <c r="D9">
-        <f>1/B9</f>
+        <f t="shared" si="0"/>
         <v>3.5069261792039282E-3</v>
       </c>
       <c r="E9">
-        <f>LOG(1/C9)</f>
+        <f t="shared" si="1"/>
         <v>-1.6020599913279623</v>
       </c>
     </row>
@@ -4824,18 +4824,18 @@
         <v>4</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>277.14999999999998</v>
       </c>
       <c r="C10">
         <v>113</v>
       </c>
       <c r="D10">
-        <f>1/B10</f>
+        <f t="shared" si="0"/>
         <v>3.608154429009562E-3</v>
       </c>
       <c r="E10">
-        <f>LOG(1/C10)</f>
+        <f t="shared" si="1"/>
         <v>-2.0530784434834199</v>
       </c>
     </row>
@@ -4844,18 +4844,18 @@
         <v>6</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>279.14999999999998</v>
       </c>
       <c r="C11">
         <v>74</v>
       </c>
       <c r="D11">
-        <f>1/B11</f>
+        <f t="shared" si="0"/>
         <v>3.5823034210997673E-3</v>
       </c>
       <c r="E11">
-        <f>LOG(1/C11)</f>
+        <f t="shared" si="1"/>
         <v>-1.8692317197309762</v>
       </c>
     </row>
@@ -4864,18 +4864,18 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>281.14999999999998</v>
       </c>
       <c r="C12">
         <v>57</v>
       </c>
       <c r="D12">
-        <f>1/B12</f>
+        <f t="shared" si="0"/>
         <v>3.556820202738752E-3</v>
       </c>
       <c r="E12">
-        <f>LOG(1/C12)</f>
+        <f t="shared" si="1"/>
         <v>-1.7558748556724915</v>
       </c>
     </row>
@@ -4884,18 +4884,18 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>283.14999999999998</v>
       </c>
       <c r="C13">
         <v>44</v>
       </c>
       <c r="D13">
-        <f>1/B13</f>
+        <f t="shared" si="0"/>
         <v>3.5316969803990822E-3</v>
       </c>
       <c r="E13">
-        <f>LOG(1/C13)</f>
+        <f t="shared" si="1"/>
         <v>-1.6434526764861874</v>
       </c>
     </row>
@@ -4904,18 +4904,18 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>285.14999999999998</v>
       </c>
       <c r="C14">
         <v>34</v>
       </c>
       <c r="D14">
-        <f>1/B14</f>
+        <f t="shared" si="0"/>
         <v>3.5069261792039282E-3</v>
       </c>
       <c r="E14">
-        <f>LOG(1/C14)</f>
+        <f t="shared" si="1"/>
         <v>-1.5314789170422551</v>
       </c>
     </row>
@@ -4924,18 +4924,18 @@
         <v>4.8</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>277.95</v>
       </c>
       <c r="C15">
         <v>115</v>
       </c>
       <c r="D15">
-        <f>1/B15</f>
+        <f t="shared" si="0"/>
         <v>3.5977693829825508E-3</v>
       </c>
       <c r="E15">
-        <f>LOG(1/C15)</f>
+        <f t="shared" si="1"/>
         <v>-2.0606978403536118</v>
       </c>
     </row>
@@ -4944,18 +4944,18 @@
         <v>6</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>279.14999999999998</v>
       </c>
       <c r="C16">
         <v>91</v>
       </c>
       <c r="D16">
-        <f>1/B16</f>
+        <f t="shared" si="0"/>
         <v>3.5823034210997673E-3</v>
       </c>
       <c r="E16">
-        <f>LOG(1/C16)</f>
+        <f t="shared" si="1"/>
         <v>-1.9590413923210936</v>
       </c>
     </row>
@@ -4964,18 +4964,18 @@
         <v>6.3</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>279.45</v>
       </c>
       <c r="C17">
         <v>87</v>
       </c>
       <c r="D17">
-        <f>1/B17</f>
+        <f t="shared" si="0"/>
         <v>3.5784576847378781E-3</v>
       </c>
       <c r="E17">
-        <f>LOG(1/C17)</f>
+        <f t="shared" si="1"/>
         <v>-1.9395192526186185</v>
       </c>
     </row>
@@ -4984,18 +4984,18 @@
         <v>6</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>279.14999999999998</v>
       </c>
       <c r="C18">
         <v>93</v>
       </c>
       <c r="D18">
-        <f>1/B18</f>
+        <f t="shared" si="0"/>
         <v>3.5823034210997673E-3</v>
       </c>
       <c r="E18">
-        <f>LOG(1/C18)</f>
+        <f t="shared" si="1"/>
         <v>-1.968482948553935</v>
       </c>
     </row>
@@ -5004,18 +5004,18 @@
         <v>6.3</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>279.45</v>
       </c>
       <c r="C19">
         <v>88</v>
       </c>
       <c r="D19">
-        <f>1/B19</f>
+        <f t="shared" si="0"/>
         <v>3.5784576847378781E-3</v>
       </c>
       <c r="E19">
-        <f>LOG(1/C19)</f>
+        <f t="shared" si="1"/>
         <v>-1.9444826721501687</v>
       </c>
     </row>
@@ -5024,18 +5024,18 @@
         <v>7.3</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>280.45</v>
       </c>
       <c r="C20">
         <v>76</v>
       </c>
       <c r="D20">
-        <f>1/B20</f>
+        <f t="shared" si="0"/>
         <v>3.5656979853806382E-3</v>
       </c>
       <c r="E20">
-        <f>LOG(1/C20)</f>
+        <f t="shared" si="1"/>
         <v>-1.8808135922807914</v>
       </c>
     </row>
@@ -5044,18 +5044,18 @@
         <v>9.4</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>282.54999999999995</v>
       </c>
       <c r="C21">
         <v>54</v>
       </c>
       <c r="D21">
-        <f>1/B21</f>
+        <f t="shared" si="0"/>
         <v>3.5391966023712623E-3</v>
       </c>
       <c r="E21">
-        <f>LOG(1/C21)</f>
+        <f t="shared" si="1"/>
         <v>-1.7323937598229686</v>
       </c>
     </row>
@@ -5064,18 +5064,18 @@
         <v>8.1</v>
       </c>
       <c r="B22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>281.25</v>
       </c>
       <c r="C22">
         <v>62</v>
       </c>
       <c r="D22">
-        <f>1/B22</f>
+        <f t="shared" si="0"/>
         <v>3.5555555555555557E-3</v>
       </c>
       <c r="E22">
-        <f>LOG(1/C22)</f>
+        <f t="shared" si="1"/>
         <v>-1.7923916894982539</v>
       </c>
     </row>
@@ -5084,18 +5084,18 @@
         <v>4.8</v>
       </c>
       <c r="B23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>277.95</v>
       </c>
       <c r="C23">
         <v>109</v>
       </c>
       <c r="D23">
-        <f>1/B23</f>
+        <f t="shared" si="0"/>
         <v>3.5977693829825508E-3</v>
       </c>
       <c r="E23">
-        <f>LOG(1/C23)</f>
+        <f t="shared" si="1"/>
         <v>-2.0374264979406238</v>
       </c>
     </row>

</xml_diff>